<commit_message>
fix boot type set ,get
</commit_message>
<xml_diff>
--- a/importexport/src/main/resources/export/booksSample.xlsx
+++ b/importexport/src/main/resources/export/booksSample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>title</t>
   </si>
@@ -39,6 +39,21 @@
   </si>
   <si>
     <t>ojojo</t>
+  </si>
+  <si>
+    <t>The Great Fire</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>Super książka</t>
+  </si>
+  <si>
+    <t>Londyn NW</t>
+  </si>
+  <si>
+    <t>Całkiem niezła</t>
   </si>
 </sst>
 </file>
@@ -99,10 +114,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.92578125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.20703125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.58984375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.03125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="7.3984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.265625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.3984375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="16.3359375" customWidth="true" bestFit="true"/>
   </cols>
@@ -161,6 +176,108 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="n">
+        <v>37723.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
+        <v>345.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="n">
+        <v>40474.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>343.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
+        <v>37723.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="n">
+        <v>345.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="n">
+        <v>40474.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="n">
+        <v>343.0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="n">
+        <v>37723.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="n">
+        <v>345.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="n">
+        <v>40474.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>343.0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
fix book type add book
</commit_message>
<xml_diff>
--- a/importexport/src/main/resources/export/booksSample.xlsx
+++ b/importexport/src/main/resources/export/booksSample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>title</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>Całkiem niezła</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>akkaka</t>
+  </si>
+  <si>
+    <t>rrea</t>
+  </si>
+  <si>
+    <t>Romance</t>
+  </si>
+  <si>
+    <t>koty</t>
   </si>
 </sst>
 </file>
@@ -117,8 +132,8 @@
     <col min="1" max="1" width="14.20703125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.58984375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.03125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="8.265625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="9.3984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.64453125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="10.375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="16.3359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -278,6 +293,74 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>37723.0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>345.0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="n">
+        <v>40474.0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="n">
+        <v>343.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="n">
+        <v>112.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.233299E7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>